<commit_message>
Add in interpretation of data
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,14 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hjjoshi/dev/glycodisplaytool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1EAAC0E-FEC7-9640-B2ED-C109FB6D6F23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB088C1-BC85-A746-B931-18FC8DE8AFB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7920" yWindow="10420" windowWidth="28040" windowHeight="17440" xr2:uid="{132FD260-0268-6D4A-A88A-BB7D1EB446EE}"/>
+    <workbookView xWindow="19220" yWindow="2280" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{132FD260-0268-6D4A-A88A-BB7D1EB446EE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test values" sheetId="1" r:id="rId1"/>
+    <sheet name="GNL" sheetId="2" r:id="rId2"/>
+    <sheet name="GSL-1" sheetId="3" r:id="rId3"/>
+    <sheet name="DSL" sheetId="4" r:id="rId4"/>
+    <sheet name="GSL-II" sheetId="5" r:id="rId5"/>
+    <sheet name="RCA-I" sheetId="7" r:id="rId6"/>
+    <sheet name="ECA" sheetId="8" r:id="rId7"/>
+    <sheet name="PHA-E" sheetId="10" r:id="rId8"/>
+    <sheet name="PHA-L" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="21">
   <si>
     <t>Cellid</t>
   </si>
@@ -64,6 +72,36 @@
   </si>
   <si>
     <t>value2</t>
+  </si>
+  <si>
+    <t>1/500</t>
+  </si>
+  <si>
+    <t>1/10000</t>
+  </si>
+  <si>
+    <t>1/5000</t>
+  </si>
+  <si>
+    <t>HEK293wt</t>
+  </si>
+  <si>
+    <t>High mannose</t>
+  </si>
+  <si>
+    <t>Tn</t>
+  </si>
+  <si>
+    <t>N-Glycan core</t>
+  </si>
+  <si>
+    <t>N-Glycan LacNAc</t>
+  </si>
+  <si>
+    <t>N-Glycan bisecting GlcNAc</t>
+  </si>
+  <si>
+    <t>1,6 branch N-glycan</t>
   </si>
 </sst>
 </file>
@@ -99,8 +137,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B37508F-C5B8-2547-BDDA-00736BA1ADCE}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,4 +571,1279 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91333FEA-4240-664F-BE02-E3383799A09A}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>17692.34</v>
+      </c>
+      <c r="C2">
+        <v>11460.47</v>
+      </c>
+      <c r="D2">
+        <v>6027.98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>775.68</v>
+      </c>
+      <c r="C3">
+        <v>443.88</v>
+      </c>
+      <c r="D3">
+        <v>387.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>721.21</v>
+      </c>
+      <c r="C4">
+        <v>426.13</v>
+      </c>
+      <c r="D4">
+        <v>356.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>19637.68</v>
+      </c>
+      <c r="C5">
+        <v>12816.7</v>
+      </c>
+      <c r="D5">
+        <v>8353.44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>17433.11</v>
+      </c>
+      <c r="C6">
+        <v>11190.63</v>
+      </c>
+      <c r="D6">
+        <v>7177.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1181.6600000000001</v>
+      </c>
+      <c r="C7">
+        <v>868.98</v>
+      </c>
+      <c r="D7">
+        <v>810.13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>22194.12</v>
+      </c>
+      <c r="C8">
+        <v>14123.05</v>
+      </c>
+      <c r="D8">
+        <v>8435.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>470.9</v>
+      </c>
+      <c r="C11">
+        <v>310.48</v>
+      </c>
+      <c r="D11">
+        <v>251.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2786AE8E-1992-1C4D-AEEB-37EB2400E873}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>305.36</v>
+      </c>
+      <c r="C2">
+        <v>282.47499999999997</v>
+      </c>
+      <c r="D2">
+        <v>205.11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1653.835</v>
+      </c>
+      <c r="C3">
+        <v>939.06500000000005</v>
+      </c>
+      <c r="D3">
+        <v>332.61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>239.23000000000002</v>
+      </c>
+      <c r="C4">
+        <v>212.06</v>
+      </c>
+      <c r="D4">
+        <v>186.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>942.35500000000002</v>
+      </c>
+      <c r="C5">
+        <v>588.29499999999996</v>
+      </c>
+      <c r="D5">
+        <v>256.76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>334.89</v>
+      </c>
+      <c r="C6">
+        <v>302.77499999999998</v>
+      </c>
+      <c r="D6">
+        <v>194.94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1804.2</v>
+      </c>
+      <c r="C7">
+        <v>1342.125</v>
+      </c>
+      <c r="D7">
+        <v>504.73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>1766.8700000000001</v>
+      </c>
+      <c r="C8">
+        <v>1010.4449999999999</v>
+      </c>
+      <c r="D8">
+        <v>415.63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3">
+        <v>187.84</v>
+      </c>
+      <c r="C11" s="3">
+        <v>169.875</v>
+      </c>
+      <c r="D11" s="3">
+        <v>155.95999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A12705-BB12-0F47-B29F-0C058CCB3ADA}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>710.28</v>
+      </c>
+      <c r="C2">
+        <v>311.36500000000001</v>
+      </c>
+      <c r="D2">
+        <v>175.45499999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>6745.5949999999993</v>
+      </c>
+      <c r="C3">
+        <v>2512.8249999999998</v>
+      </c>
+      <c r="D3">
+        <v>580.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>6690.01</v>
+      </c>
+      <c r="C4">
+        <v>2267.2600000000002</v>
+      </c>
+      <c r="D4">
+        <v>500.02499999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>866.28500000000008</v>
+      </c>
+      <c r="C5">
+        <v>369.95500000000004</v>
+      </c>
+      <c r="D5">
+        <v>202.785</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>201.01499999999999</v>
+      </c>
+      <c r="C6">
+        <v>150.78500000000003</v>
+      </c>
+      <c r="D6">
+        <v>135.535</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>8899.84</v>
+      </c>
+      <c r="C7">
+        <v>3561.9449999999997</v>
+      </c>
+      <c r="D7">
+        <v>1452.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>358.56</v>
+      </c>
+      <c r="C8">
+        <v>231.56</v>
+      </c>
+      <c r="D8">
+        <v>199.51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>7434.8250000000007</v>
+      </c>
+      <c r="C11">
+        <v>2473.6400000000003</v>
+      </c>
+      <c r="D11">
+        <v>583.79500000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A418D3DE-2B21-5A4B-BD73-B1FD8C08BFA2}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>351.34500000000003</v>
+      </c>
+      <c r="C2">
+        <v>330.69499999999999</v>
+      </c>
+      <c r="D2">
+        <v>233.80500000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>239.685</v>
+      </c>
+      <c r="C3">
+        <v>221.74</v>
+      </c>
+      <c r="D3">
+        <v>228.44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>186.39</v>
+      </c>
+      <c r="C4">
+        <v>188.285</v>
+      </c>
+      <c r="D4">
+        <v>188.23500000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>367.11500000000001</v>
+      </c>
+      <c r="C5">
+        <v>335.7</v>
+      </c>
+      <c r="D5">
+        <v>233.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>355.37</v>
+      </c>
+      <c r="C6">
+        <v>329.97500000000002</v>
+      </c>
+      <c r="D6">
+        <v>217.17500000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>934.12999999999988</v>
+      </c>
+      <c r="C7">
+        <v>946.32999999999993</v>
+      </c>
+      <c r="D7">
+        <v>922.14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>454.63</v>
+      </c>
+      <c r="C8">
+        <v>402.85</v>
+      </c>
+      <c r="D8">
+        <v>274.40999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>159.95500000000001</v>
+      </c>
+      <c r="C11">
+        <v>152.78500000000003</v>
+      </c>
+      <c r="D11">
+        <v>207.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDD852F-5DC4-CD44-A960-14F5161ACEEF}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>21416.165000000001</v>
+      </c>
+      <c r="C2">
+        <v>9201.26</v>
+      </c>
+      <c r="D2">
+        <v>5585.5749999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>70036.014999999999</v>
+      </c>
+      <c r="C3">
+        <v>47066.164999999994</v>
+      </c>
+      <c r="D3">
+        <v>31493.38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>55845.41</v>
+      </c>
+      <c r="C4">
+        <v>41502.649999999994</v>
+      </c>
+      <c r="D4">
+        <v>30266.300000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>20020.745000000003</v>
+      </c>
+      <c r="C5">
+        <v>7913.9699999999993</v>
+      </c>
+      <c r="D5">
+        <v>3974.1099999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>3150.5749999999998</v>
+      </c>
+      <c r="C6">
+        <v>1581.895</v>
+      </c>
+      <c r="D6">
+        <v>956.37000000000012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>60951.61</v>
+      </c>
+      <c r="C7">
+        <v>43573.304999999993</v>
+      </c>
+      <c r="D7">
+        <v>33778.410000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>3991.26</v>
+      </c>
+      <c r="C8">
+        <v>1649.8049999999998</v>
+      </c>
+      <c r="D8">
+        <v>1050.42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>66354.554999999993</v>
+      </c>
+      <c r="C11">
+        <v>39191.35</v>
+      </c>
+      <c r="D11">
+        <v>29948.760000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0517DA99-2F53-9448-84CF-9FA7BED736B1}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>10414.52</v>
+      </c>
+      <c r="C2">
+        <v>1284.825</v>
+      </c>
+      <c r="D2">
+        <v>645.79999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>30589.269999999997</v>
+      </c>
+      <c r="C3">
+        <v>6776.53</v>
+      </c>
+      <c r="D3">
+        <v>3844.2550000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>37217.9</v>
+      </c>
+      <c r="C4">
+        <v>8145.0650000000005</v>
+      </c>
+      <c r="D4">
+        <v>4422.5349999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>9190.1350000000002</v>
+      </c>
+      <c r="C5">
+        <v>845.57500000000005</v>
+      </c>
+      <c r="D5">
+        <v>484.54999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>898.41499999999996</v>
+      </c>
+      <c r="C6">
+        <v>341.61</v>
+      </c>
+      <c r="D6">
+        <v>236.32500000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>37079.584999999999</v>
+      </c>
+      <c r="C7">
+        <v>9253.3450000000012</v>
+      </c>
+      <c r="D7">
+        <v>5523.3600000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>832.875</v>
+      </c>
+      <c r="C8">
+        <v>356.67500000000001</v>
+      </c>
+      <c r="D8">
+        <v>275.745</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>43932.875</v>
+      </c>
+      <c r="C11">
+        <v>9207.65</v>
+      </c>
+      <c r="D11">
+        <v>5073.0750000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BACF9B-2897-7D42-8317-6BFC6676044B}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>241.35500000000002</v>
+      </c>
+      <c r="C2">
+        <v>193.56</v>
+      </c>
+      <c r="D2">
+        <v>178.37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>40359.47</v>
+      </c>
+      <c r="C3">
+        <v>15699.155000000001</v>
+      </c>
+      <c r="D3">
+        <v>8420.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>38158.384999999995</v>
+      </c>
+      <c r="C4">
+        <v>15281.68</v>
+      </c>
+      <c r="D4">
+        <v>8398.5849999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>268.13499999999999</v>
+      </c>
+      <c r="C5">
+        <v>207.54500000000002</v>
+      </c>
+      <c r="D5">
+        <v>189.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>216.53</v>
+      </c>
+      <c r="C6">
+        <v>168.79500000000002</v>
+      </c>
+      <c r="D6">
+        <v>152.67500000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>39877.08</v>
+      </c>
+      <c r="C7">
+        <v>15723.24</v>
+      </c>
+      <c r="D7">
+        <v>8962.8649999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>248.965</v>
+      </c>
+      <c r="C8">
+        <v>212.16</v>
+      </c>
+      <c r="D8">
+        <v>199.39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>35214.345000000001</v>
+      </c>
+      <c r="C11">
+        <v>13348.01</v>
+      </c>
+      <c r="D11">
+        <v>7266.5749999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA31A37-4399-4643-ADB1-551B189B1132}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>151</v>
+      </c>
+      <c r="C2">
+        <v>148.32</v>
+      </c>
+      <c r="D2">
+        <v>140.81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>20418.79</v>
+      </c>
+      <c r="C3">
+        <v>12218.25</v>
+      </c>
+      <c r="D3">
+        <v>6698.52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>19382.43</v>
+      </c>
+      <c r="C4">
+        <v>9564.6200000000008</v>
+      </c>
+      <c r="D4">
+        <v>5306.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>168.87</v>
+      </c>
+      <c r="C5">
+        <v>163.13</v>
+      </c>
+      <c r="D5">
+        <v>164.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>131.56</v>
+      </c>
+      <c r="C6">
+        <v>122.85</v>
+      </c>
+      <c r="D6">
+        <v>124.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>19436.509999999998</v>
+      </c>
+      <c r="C7">
+        <v>13657.91</v>
+      </c>
+      <c r="D7">
+        <v>8217.7199999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>197.28</v>
+      </c>
+      <c r="C8">
+        <v>194.58</v>
+      </c>
+      <c r="D8">
+        <v>191.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>18319.75</v>
+      </c>
+      <c r="C11">
+        <v>10790.56</v>
+      </c>
+      <c r="D11">
+        <v>5827.98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>